<commit_message>
feat: updated sprint backlogs
</commit_message>
<xml_diff>
--- a/Sprint Backlogs, Sprint 1 and 2.xlsx
+++ b/Sprint Backlogs, Sprint 1 and 2.xlsx
@@ -71,12 +71,15 @@
     <t>Done</t>
   </si>
   <si>
-    <t>Target: get done by Sprint 2 (work on now as well)</t>
+    <t>Target: get done by Sprint 2 (work on now as well). 0 points left?</t>
   </si>
   <si>
     <t>Recommended locations should be near previously-traveled locations</t>
   </si>
   <si>
+    <t>Target: get done by Sprint 2 (work on now as well). 5 points left?</t>
+  </si>
+  <si>
     <t>User Story #2</t>
   </si>
   <si>
@@ -86,6 +89,9 @@
     <t>Display travel options at cheaper price points</t>
   </si>
   <si>
+    <t>Target: get done by Sprint 2 (work on now as well). 2 points left?</t>
+  </si>
+  <si>
     <t>Display travel cheaper price combinations for travel (flight, hotel, destination)</t>
   </si>
   <si>
@@ -98,7 +104,7 @@
     <t>Allow users to select their desired hotel to stay at during their travel.</t>
   </si>
   <si>
-    <t>Target: get done by Sprint 1 - some rework needed, finish early in Sprint 2</t>
+    <t>Target: get done by Sprint 1 - some rework needed, finish early in Sprint 2. 5 points left?</t>
   </si>
   <si>
     <t>Allow users to select whether they would like to travel by plane or not.</t>
@@ -131,9 +137,6 @@
     <t>Estimated Effort (left)</t>
   </si>
   <si>
-    <t>Recommend new travel destinations based on previous travel,  debugging recommender system</t>
-  </si>
-  <si>
     <t>Target: get done by Sprint 2 - Done</t>
   </si>
   <si>
@@ -147,9 +150,6 @@
   </si>
   <si>
     <t>All</t>
-  </si>
-  <si>
-    <t>Target: get done by Sprint 2</t>
   </si>
   <si>
     <t>Generally debug code, testing</t>
@@ -159,7 +159,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -199,6 +199,11 @@
       <sz val="11.0"/>
       <color rgb="FFB7B7B7"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -330,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -400,6 +405,9 @@
     <xf borderId="8" fillId="6" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="8" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -725,7 +733,7 @@
         <v>7.0</v>
       </c>
       <c r="H4" s="13">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="I4" s="13">
         <v>0.0</v>
@@ -746,7 +754,7 @@
       <c r="B5" s="17"/>
       <c r="C5" s="18"/>
       <c r="D5" s="19">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
       <c r="E5" s="19">
         <v>3.0</v>
@@ -755,7 +763,7 @@
         <v>0.0</v>
       </c>
       <c r="G5" s="19">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="H5" s="19">
         <v>1.0</v>
@@ -780,7 +788,7 @@
       <c r="B6" s="17"/>
       <c r="C6" s="18"/>
       <c r="D6" s="19">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="E6" s="19">
         <v>0.0</v>
@@ -792,7 +800,7 @@
         <v>2.0</v>
       </c>
       <c r="H6" s="19">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="I6" s="19">
         <v>0.0</v>
@@ -804,7 +812,7 @@
         <v>16</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
@@ -837,13 +845,13 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B9" s="23">
         <v>12.0</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9" s="13">
         <v>8.0</v>
@@ -873,7 +881,7 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="18"/>
@@ -902,12 +910,12 @@
         <v>16</v>
       </c>
       <c r="L10" s="21" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B11" s="17"/>
       <c r="C11" s="18"/>
@@ -936,7 +944,7 @@
         <v>16</v>
       </c>
       <c r="L11" s="21" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
@@ -969,31 +977,31 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B14" s="23">
         <v>14.0</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D14" s="13">
         <v>14.0</v>
       </c>
       <c r="E14" s="13">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="F14" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="G14" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="H14" s="13">
+        <v>0.0</v>
+      </c>
+      <c r="I14" s="13">
         <v>2.0</v>
-      </c>
-      <c r="G14" s="13">
-        <v>4.0</v>
-      </c>
-      <c r="H14" s="13">
-        <v>0.0</v>
-      </c>
-      <c r="I14" s="13">
-        <v>3.0</v>
       </c>
       <c r="J14" s="13">
         <v>0.0</v>
@@ -1005,18 +1013,18 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="16" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="18"/>
       <c r="D15" s="19">
-        <v>15.0</v>
+        <v>9.0</v>
       </c>
       <c r="E15" s="19">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="F15" s="19">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="G15" s="20">
         <v>0.0</v>
@@ -1034,12 +1042,12 @@
         <v>16</v>
       </c>
       <c r="L15" s="21" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="16" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B16" s="17"/>
       <c r="C16" s="18"/>
@@ -1053,13 +1061,13 @@
         <v>0.0</v>
       </c>
       <c r="G16" s="19">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="H16" s="19">
         <v>0.0</v>
       </c>
       <c r="I16" s="19">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="J16" s="19">
         <v>0.0</v>
@@ -1068,7 +1076,7 @@
         <v>18</v>
       </c>
       <c r="L16" s="21" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
@@ -1101,13 +1109,13 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B19" s="23">
         <v>12.0</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D19" s="13">
         <v>12.0</v>
@@ -1138,7 +1146,7 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="16" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="18"/>
@@ -1165,12 +1173,12 @@
         <v>18</v>
       </c>
       <c r="L20" s="21" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="18"/>
@@ -1199,7 +1207,7 @@
         <v>18</v>
       </c>
       <c r="L21" s="21" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
@@ -1232,7 +1240,7 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="24" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B24" s="23"/>
       <c r="C24" s="14"/>
@@ -1304,7 +1312,7 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="27" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B29" s="28"/>
       <c r="C29" s="28"/>
@@ -1314,23 +1322,23 @@
       </c>
       <c r="E29" s="29">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F29" s="29">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G29" s="29">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H29" s="29">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I29" s="29">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J29" s="29">
         <f t="shared" si="1"/>
@@ -2381,13 +2389,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>6</v>
@@ -2431,10 +2439,10 @@
         <v>1.0</v>
       </c>
       <c r="F4" s="13">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="G4" s="13">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H4" s="13">
         <v>0.0</v>
@@ -2443,7 +2451,7 @@
         <v>0.0</v>
       </c>
       <c r="J4" s="14">
-        <f>SUM(J5:J8)</f>
+        <f>SUM(J6:J8)</f>
         <v>0</v>
       </c>
       <c r="K4" s="15" t="s">
@@ -2453,56 +2461,69 @@
     </row>
     <row r="5">
       <c r="A5" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="17"/>
+        <v>17</v>
+      </c>
       <c r="C5" s="18"/>
-      <c r="D5" s="19">
-        <v>5.0</v>
-      </c>
-      <c r="E5" s="19">
-        <v>1.0</v>
-      </c>
-      <c r="F5" s="19">
-        <v>3.0</v>
-      </c>
-      <c r="G5" s="19">
-        <v>1.0</v>
-      </c>
-      <c r="H5" s="19">
-        <v>0.0</v>
-      </c>
-      <c r="I5" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="J5" s="20">
+      <c r="D5" s="30">
+        <v>0.0</v>
+      </c>
+      <c r="E5" s="30">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="30">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="30">
+        <v>0.0</v>
+      </c>
+      <c r="H5" s="30">
+        <v>0.0</v>
+      </c>
+      <c r="I5" s="30">
+        <v>0.0</v>
+      </c>
+      <c r="J5" s="30">
         <v>0.0</v>
       </c>
       <c r="K5" s="15" t="s">
         <v>18</v>
       </c>
       <c r="L5" s="21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="16" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B6" s="17"/>
       <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="20"/>
+      <c r="D6" s="19">
+        <v>5.0</v>
+      </c>
+      <c r="E6" s="19">
+        <v>1.0</v>
+      </c>
+      <c r="F6" s="19">
+        <v>2.0</v>
+      </c>
+      <c r="G6" s="19">
+        <v>2.0</v>
+      </c>
+      <c r="H6" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="I6" s="20">
+        <v>0.0</v>
+      </c>
+      <c r="J6" s="20">
+        <v>0.0</v>
+      </c>
       <c r="K6" s="15" t="s">
         <v>18</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7">
@@ -2535,13 +2556,13 @@
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B9" s="23">
         <v>12.0</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9" s="13">
         <v>4.0</v>
@@ -2553,7 +2574,7 @@
         <v>0.0</v>
       </c>
       <c r="G9" s="13">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H9" s="13">
         <v>0.0</v>
@@ -2571,12 +2592,12 @@
     </row>
     <row r="10">
       <c r="A10" s="16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="18"/>
       <c r="D10" s="19">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E10" s="19">
         <v>1.0</v>
@@ -2585,7 +2606,7 @@
         <v>0.0</v>
       </c>
       <c r="G10" s="19">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H10" s="19">
         <v>0.0</v>
@@ -2600,20 +2621,20 @@
         <v>18</v>
       </c>
       <c r="L10" s="21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B11" s="17"/>
       <c r="C11" s="18"/>
       <c r="D11" s="19">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="E11" s="19">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="F11" s="19">
         <v>0.0</v>
@@ -2634,7 +2655,7 @@
         <v>18</v>
       </c>
       <c r="L11" s="21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12">
@@ -2667,13 +2688,13 @@
     </row>
     <row r="14">
       <c r="A14" s="10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B14" s="23">
         <v>14.0</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D14" s="13">
         <v>5.0</v>
@@ -2703,7 +2724,7 @@
     </row>
     <row r="15">
       <c r="A15" s="16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="18"/>
@@ -2732,7 +2753,7 @@
         <v>18</v>
       </c>
       <c r="L15" s="21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16">
@@ -2746,7 +2767,7 @@
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
       <c r="J16" s="19"/>
-      <c r="K16" s="30"/>
+      <c r="K16" s="31"/>
       <c r="L16" s="19"/>
     </row>
     <row r="17">
@@ -2779,13 +2800,13 @@
     </row>
     <row r="19">
       <c r="A19" s="10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B19" s="23">
         <v>12.0</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D19" s="13">
         <v>0.0</v>
@@ -2816,7 +2837,7 @@
     </row>
     <row r="20">
       <c r="A20" s="16" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="18"/>
@@ -2836,7 +2857,7 @@
     </row>
     <row r="21">
       <c r="A21" s="16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="18"/>
@@ -2884,7 +2905,7 @@
     </row>
     <row r="24">
       <c r="A24" s="24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B24" s="23"/>
       <c r="C24" s="14"/>
@@ -2914,11 +2935,11 @@
     </row>
     <row r="25">
       <c r="A25" s="16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B25" s="25"/>
       <c r="C25" s="26" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D25" s="19">
         <v>8.0</v>
@@ -2945,7 +2966,7 @@
         <v>18</v>
       </c>
       <c r="L25" s="21" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26">
@@ -2954,7 +2975,7 @@
       </c>
       <c r="B26" s="25"/>
       <c r="C26" s="26" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D26" s="19">
         <v>16.0</v>
@@ -2981,7 +3002,7 @@
         <v>18</v>
       </c>
       <c r="L26" s="21" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27">
@@ -3014,7 +3035,7 @@
     </row>
     <row r="29">
       <c r="A29" s="27" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B29" s="28"/>
       <c r="C29" s="28"/>
@@ -3028,11 +3049,11 @@
       </c>
       <c r="F29" s="29">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G29" s="29">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H29" s="29">
         <f t="shared" si="1"/>

</xml_diff>